<commit_message>
making patterns for ulna
</commit_message>
<xml_diff>
--- a/terms/oba_toDO.xlsx
+++ b/terms/oba_toDO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231137CA-4F23-B949-8CF5-85506682F3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46513094-CE19-4646-8B25-98DC4DA09F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7880" yWindow="3920" windowWidth="27240" windowHeight="15640" xr2:uid="{28C3DE2E-F2D6-784F-BFCF-470921B0D866}"/>
+    <workbookView xWindow="1560" yWindow="1500" windowWidth="27240" windowHeight="15640" xr2:uid="{28C3DE2E-F2D6-784F-BFCF-470921B0D866}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>improve equivalency for</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>humerus</t>
+  </si>
+  <si>
+    <t>ulna</t>
+  </si>
+  <si>
+    <t>radius</t>
   </si>
 </sst>
 </file>
@@ -394,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B2E0B7-6799-F140-BF4C-F6E5AB62C570}">
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -430,6 +436,16 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>